<commit_message>
Added all tests. Added new scenarios to Chart
</commit_message>
<xml_diff>
--- a/Project2 Data Spreadsheet & Chart_v1.xlsx
+++ b/Project2 Data Spreadsheet & Chart_v1.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derekfinlinson\git\6310TeamProject2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="25660" windowHeight="16600"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="25665" windowHeight="16605" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Time" sheetId="1" r:id="rId1"/>
     <sheet name="Memory" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="18">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -83,6 +88,21 @@
       </rPr>
       <t>1</t>
     </r>
+  </si>
+  <si>
+    <t>Grid = 15, Sim Rate = 10, Vis Rate = 1</t>
+  </si>
+  <si>
+    <t>Scenario 6</t>
+  </si>
+  <si>
+    <t>Scenario 7</t>
+  </si>
+  <si>
+    <t>Grid = 15, Sim Rate = 10, Vis Rate = 3</t>
+  </si>
+  <si>
+    <t>Grid = 15, Sim Rate = 5, Vis Rate = 1</t>
   </si>
 </sst>
 </file>
@@ -187,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -204,12 +224,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -259,7 +290,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$2</c:f>
+              <c:f>Time!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -271,7 +302,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$1:$E$1</c:f>
+              <c:f>Time!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -291,7 +322,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$2:$E$2</c:f>
+              <c:f>Time!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -304,7 +335,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$3</c:f>
+              <c:f>Time!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +347,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$1:$E$1</c:f>
+              <c:f>Time!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -336,7 +367,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$3:$E$3</c:f>
+              <c:f>Time!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -349,7 +380,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$4</c:f>
+              <c:f>Time!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -361,7 +392,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$1:$E$1</c:f>
+              <c:f>Time!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -381,7 +412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$4:$E$4</c:f>
+              <c:f>Time!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -398,20 +429,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124093048"/>
-        <c:axId val="2112215480"/>
+        <c:axId val="443744520"/>
+        <c:axId val="443742168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124093048"/>
+        <c:axId val="443744520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112215480"/>
+        <c:crossAx val="443742168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -419,7 +451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112215480"/>
+        <c:axId val="443742168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +462,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124093048"/>
+        <c:crossAx val="443744520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -477,6 +509,486 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Memory Usage (Scenario 3)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Push –t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$15:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pull –r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$16:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffered –b 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$17:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="443748832"/>
+        <c:axId val="443752752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="443748832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="443752752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="443752752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="443748832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Memory Usage (Scenario 4)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Push –t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$20:$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$21:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pull –r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$20:$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$22:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffered –b 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$20:$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$23:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="443753144"/>
+        <c:axId val="443753536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="443753144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="443753536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="443753536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="443753144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
               <a:t>Memory Usage (Scenario 5)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
@@ -498,7 +1010,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$22</c:f>
+              <c:f>Memory!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -510,7 +1022,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$21:$E$21</c:f>
+              <c:f>Memory!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -530,7 +1042,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$22:$E$22</c:f>
+              <c:f>Memory!$B$27:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -543,7 +1055,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$23</c:f>
+              <c:f>Memory!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -555,7 +1067,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$21:$E$21</c:f>
+              <c:f>Memory!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -575,7 +1087,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$23:$E$23</c:f>
+              <c:f>Memory!$B$28:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -588,7 +1100,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$24</c:f>
+              <c:f>Memory!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -600,7 +1112,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$21:$E$21</c:f>
+              <c:f>Memory!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -620,7 +1132,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$24:$E$24</c:f>
+              <c:f>Memory!$B$29:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -637,20 +1149,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060469480"/>
-        <c:axId val="-2061026872"/>
+        <c:axId val="443759024"/>
+        <c:axId val="443756280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060469480"/>
+        <c:axId val="443759024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061026872"/>
+        <c:crossAx val="443756280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -658,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061026872"/>
+        <c:axId val="443756280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +1182,487 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060469480"/>
+        <c:crossAx val="443759024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Memory Usage (Scenario 6)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Push –t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$32:$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$33:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pull –r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$32:$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$34:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffered –b 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$32:$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$35:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="273583368"/>
+        <c:axId val="273586896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="273583368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="273586896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="273586896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="273583368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Memory Usage (Scenario 7)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Push –t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$38:$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$39:$E$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pull –r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$38:$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$40:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffered –b 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Memory!$B$38:$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Memory!$B$41:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="255403360"/>
+        <c:axId val="255399048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="255403360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="255399048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="255399048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="255403360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,7 +1729,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$7</c:f>
+              <c:f>Time!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -748,7 +1741,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$6:$E$6</c:f>
+              <c:f>Time!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -768,7 +1761,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$7:$E$7</c:f>
+              <c:f>Time!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -781,7 +1774,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$8</c:f>
+              <c:f>Time!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -793,7 +1786,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$6:$E$6</c:f>
+              <c:f>Time!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -813,7 +1806,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$8:$E$8</c:f>
+              <c:f>Time!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -826,7 +1819,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$9</c:f>
+              <c:f>Time!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -838,7 +1831,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$6:$E$6</c:f>
+              <c:f>Time!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -858,7 +1851,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$9:$E$9</c:f>
+              <c:f>Time!$B$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -875,20 +1868,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060739896"/>
-        <c:axId val="-2060736920"/>
+        <c:axId val="443752360"/>
+        <c:axId val="443741384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060739896"/>
+        <c:axId val="443752360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060736920"/>
+        <c:crossAx val="443741384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -896,7 +1890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060736920"/>
+        <c:axId val="443741384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +1901,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060739896"/>
+        <c:crossAx val="443752360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -974,7 +1968,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$12</c:f>
+              <c:f>Time!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -986,7 +1980,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$11:$E$11</c:f>
+              <c:f>Time!$B$14:$E$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1006,7 +2000,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$12:$E$12</c:f>
+              <c:f>Time!$B$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1019,7 +2013,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$13</c:f>
+              <c:f>Time!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1031,7 +2025,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$11:$E$11</c:f>
+              <c:f>Time!$B$14:$E$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1051,7 +2045,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$13:$E$13</c:f>
+              <c:f>Time!$B$16:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1064,7 +2058,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$14</c:f>
+              <c:f>Time!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1076,7 +2070,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$11:$E$11</c:f>
+              <c:f>Time!$B$14:$E$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1096,7 +2090,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$14:$E$14</c:f>
+              <c:f>Time!$B$17:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1113,20 +2107,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060699960"/>
-        <c:axId val="-2060696984"/>
+        <c:axId val="443746872"/>
+        <c:axId val="443742952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060699960"/>
+        <c:axId val="443746872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060696984"/>
+        <c:crossAx val="443742952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1134,7 +2129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060696984"/>
+        <c:axId val="443742952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +2140,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060699960"/>
+        <c:crossAx val="443746872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1197,7 +2192,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1212,7 +2206,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$17</c:f>
+              <c:f>Time!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1224,7 +2218,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$16:$E$16</c:f>
+              <c:f>Time!$B$20:$E$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1244,7 +2238,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$17:$E$17</c:f>
+              <c:f>Time!$B$21:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1257,7 +2251,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$18</c:f>
+              <c:f>Time!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1269,7 +2263,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$16:$E$16</c:f>
+              <c:f>Time!$B$20:$E$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1289,7 +2283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$18:$E$18</c:f>
+              <c:f>Time!$B$22:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1302,7 +2296,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$19</c:f>
+              <c:f>Time!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1314,7 +2308,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$16:$E$16</c:f>
+              <c:f>Time!$B$20:$E$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1334,7 +2328,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$19:$E$19</c:f>
+              <c:f>Time!$B$23:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1351,20 +2345,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060663256"/>
-        <c:axId val="-2060660280"/>
+        <c:axId val="443747264"/>
+        <c:axId val="443740208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060663256"/>
+        <c:axId val="443747264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060660280"/>
+        <c:crossAx val="443740208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1372,7 +2367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060660280"/>
+        <c:axId val="443740208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,14 +2378,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060663256"/>
+        <c:crossAx val="443747264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1445,11 +2439,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$22</c:f>
+              <c:f>Time!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1461,7 +2455,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$21:$E$21</c:f>
+              <c:f>Time!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1481,7 +2475,142 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$22:$E$22</c:f>
+              <c:f>Time!$B$27:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pull –r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Time!$B$26:$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Time!$B$28:$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffered –b 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Time!$B$26:$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Time!$B$29:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Push –t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Time!$B$26:$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Non-Threaded</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Simulation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Presentation Threaded</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Both Threaded -s -p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Time!$B$27:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1491,10 +2620,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$23</c:f>
+              <c:f>Time!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1506,7 +2635,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$21:$E$21</c:f>
+              <c:f>Time!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1526,7 +2655,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$23:$E$23</c:f>
+              <c:f>Time!$B$28:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1536,10 +2665,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$A$24</c:f>
+              <c:f>Time!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1551,7 +2680,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Time!$B$21:$E$21</c:f>
+              <c:f>Time!$B$26:$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1571,7 +2700,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Time!$B$24:$E$24</c:f>
+              <c:f>Time!$B$29:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1588,20 +2717,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060625688"/>
-        <c:axId val="-2060622712"/>
+        <c:axId val="443740992"/>
+        <c:axId val="443750008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060625688"/>
+        <c:axId val="443740992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060622712"/>
+        <c:crossAx val="443750008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1609,7 +2739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060622712"/>
+        <c:axId val="443750008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,7 +2750,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060625688"/>
+        <c:crossAx val="443740992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1666,12 +2796,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Memory Usage (Scenario 1)</a:t>
+              <a:t>Time of execution (Scenario 6)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8375871119558273E-3"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1686,7 +2823,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$2</c:f>
+              <c:f>Time!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1698,7 +2835,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$1:$E$1</c:f>
+              <c:f>Time!$B$32:$E$32</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1718,7 +2855,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$2:$E$2</c:f>
+              <c:f>Time!$B$33:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1731,7 +2868,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$3</c:f>
+              <c:f>Time!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1743,7 +2880,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$1:$E$1</c:f>
+              <c:f>Time!$B$32:$E$32</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1763,7 +2900,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$3:$E$3</c:f>
+              <c:f>Time!$B$34:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1776,7 +2913,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$4</c:f>
+              <c:f>Time!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1788,7 +2925,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$1:$E$1</c:f>
+              <c:f>Time!$B$32:$E$32</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1808,7 +2945,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$4:$E$4</c:f>
+              <c:f>Time!$B$35:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1825,20 +2962,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2133697336"/>
-        <c:axId val="2133700312"/>
+        <c:axId val="443745696"/>
+        <c:axId val="443741776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133697336"/>
+        <c:axId val="443745696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133700312"/>
+        <c:crossAx val="443741776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1846,7 +2984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133700312"/>
+        <c:axId val="443741776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1857,14 +2995,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133697336"/>
+        <c:crossAx val="443745696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1904,13 +3041,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Memory Usage (Scenario 2)</a:t>
+              <a:t>Time of execution (Scenario 7)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8375871119558273E-3"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1925,7 +3068,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$7</c:f>
+              <c:f>Time!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1937,7 +3080,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$6:$E$6</c:f>
+              <c:f>Time!$B$38:$E$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1957,7 +3100,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$7:$E$7</c:f>
+              <c:f>Time!$B$39:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1970,7 +3113,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$8</c:f>
+              <c:f>Time!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1982,7 +3125,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$6:$E$6</c:f>
+              <c:f>Time!$B$38:$E$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2002,7 +3145,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$8:$E$8</c:f>
+              <c:f>Time!$B$40:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2015,7 +3158,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$9</c:f>
+              <c:f>Time!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2027,7 +3170,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$6:$E$6</c:f>
+              <c:f>Time!$B$38:$E$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2047,7 +3190,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$9:$E$9</c:f>
+              <c:f>Time!$B$41:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2064,20 +3207,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060582808"/>
-        <c:axId val="-2060579832"/>
+        <c:axId val="443746088"/>
+        <c:axId val="443750400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060582808"/>
+        <c:axId val="443746088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060579832"/>
+        <c:crossAx val="443750400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2085,7 +3229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060579832"/>
+        <c:axId val="443750400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,14 +3240,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060582808"/>
+        <c:crossAx val="443746088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2143,9 +3286,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Memory Usage (Scenario 3)</a:t>
+              <a:t>Memory Usage (Scenario 1)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2164,7 +3306,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$12</c:f>
+              <c:f>Memory!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2176,7 +3318,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$11:$E$11</c:f>
+              <c:f>Memory!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2196,7 +3338,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$12:$E$12</c:f>
+              <c:f>Memory!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2209,7 +3351,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$13</c:f>
+              <c:f>Memory!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2221,7 +3363,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$11:$E$11</c:f>
+              <c:f>Memory!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2241,7 +3383,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$13:$E$13</c:f>
+              <c:f>Memory!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2254,7 +3396,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$14</c:f>
+              <c:f>Memory!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2266,7 +3408,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$11:$E$11</c:f>
+              <c:f>Memory!$B$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2286,7 +3428,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$14:$E$14</c:f>
+              <c:f>Memory!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2303,20 +3445,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060545336"/>
-        <c:axId val="-2060542360"/>
+        <c:axId val="443751184"/>
+        <c:axId val="443751576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060545336"/>
+        <c:axId val="443751184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060542360"/>
+        <c:crossAx val="443751576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2324,7 +3467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060542360"/>
+        <c:axId val="443751576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,7 +3478,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060545336"/>
+        <c:crossAx val="443751184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2382,7 +3525,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Memory Usage (Scenario 4)</a:t>
+              <a:t>Memory Usage (Scenario 2)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2403,7 +3546,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$17</c:f>
+              <c:f>Memory!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2415,7 +3558,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$16:$E$16</c:f>
+              <c:f>Memory!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2435,7 +3578,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$17:$E$17</c:f>
+              <c:f>Memory!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2448,7 +3591,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$18</c:f>
+              <c:f>Memory!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2460,7 +3603,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$16:$E$16</c:f>
+              <c:f>Memory!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2480,7 +3623,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$18:$E$18</c:f>
+              <c:f>Memory!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2493,7 +3636,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$A$19</c:f>
+              <c:f>Memory!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2505,7 +3648,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Memory!$B$16:$E$16</c:f>
+              <c:f>Memory!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2525,7 +3668,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Memory!$B$19:$E$19</c:f>
+              <c:f>Memory!$B$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2542,20 +3685,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2060507816"/>
-        <c:axId val="-2060504840"/>
+        <c:axId val="443755888"/>
+        <c:axId val="443759808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2060507816"/>
+        <c:axId val="443755888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060504840"/>
+        <c:crossAx val="443759808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2563,7 +3707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060504840"/>
+        <c:axId val="443759808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2574,7 +3718,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2060507816"/>
+        <c:crossAx val="443755888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2602,13 +3746,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2632,13 +3776,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2662,13 +3806,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2692,13 +3836,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2722,13 +3866,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2748,6 +3892,70 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2757,13 +3965,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2787,13 +3995,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>371475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2817,13 +4025,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2847,13 +4055,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2877,13 +4085,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2898,6 +4106,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3191,244 +4463,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1"/>
-    <row r="6" spans="1:5" ht="31" thickBot="1">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1"/>
-    <row r="11" spans="1:5" ht="31" thickBot="1">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" thickBot="1">
-      <c r="A12" s="3" t="s">
+    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
-      <c r="A13" s="3" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1">
-      <c r="A14" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1"/>
-    <row r="16" spans="1:5" ht="31" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="16" thickBot="1">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="16" thickBot="1">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1"/>
-    <row r="21" spans="1:5" ht="31" thickBot="1">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" thickBot="1">
-      <c r="A22" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="16" thickBot="1">
-      <c r="A23" s="3" t="s">
-        <v>6</v>
+    <row r="23" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3444,244 +4833,363 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1"/>
-    <row r="6" spans="1:5" ht="31" thickBot="1">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1"/>
-    <row r="11" spans="1:5" ht="31" thickBot="1">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" thickBot="1">
-      <c r="A12" s="3" t="s">
+    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
-      <c r="A13" s="3" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1">
-      <c r="A14" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1"/>
-    <row r="16" spans="1:5" ht="31" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="16" thickBot="1">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="16" thickBot="1">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1"/>
-    <row r="21" spans="1:5" ht="31" thickBot="1">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" thickBot="1">
-      <c r="A22" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="16" thickBot="1">
-      <c r="A23" s="3" t="s">
-        <v>6</v>
+    <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>